<commit_message>
Ajout du guide Sigfox
</commit_message>
<xml_diff>
--- a/001 - Embarquement/Identifiants.xlsx
+++ b/001 - Embarquement/Identifiants.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reynh\LACROIX GROUP\LACROIX GROUP\Atelier Arduino LPWAN - General\LACROIX-Lab-Atelier-Arduino\001 - Embarquement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lacroixgroup.sharepoint.com/sites/AtelierArduinoLPWAN/Documents partages/General/LACROIX-Lab-Atelier-Arduino/001 - Embarquement/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10350" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10350"/>
   </bookViews>
   <sheets>
     <sheet name="LoRa" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Device EUI</t>
   </si>
@@ -227,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -236,6 +236,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,21 +596,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.86328125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -625,7 +627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -642,7 +644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -659,31 +661,40 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="9">
+        <v>64754638</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -691,7 +702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1</v>
       </c>
@@ -699,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>2</v>
       </c>
@@ -707,7 +718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>3</v>
       </c>
@@ -715,7 +726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>4</v>
       </c>
@@ -723,7 +734,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>5</v>
       </c>
@@ -731,7 +742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>6</v>
       </c>
@@ -739,7 +750,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>7</v>
       </c>
@@ -760,16 +771,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -783,7 +794,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1</v>
       </c>
@@ -797,7 +808,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2</v>
       </c>
@@ -811,7 +822,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>3</v>
       </c>
@@ -825,7 +836,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>4</v>
       </c>
@@ -839,7 +850,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>5</v>
       </c>
@@ -853,7 +864,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>6</v>
       </c>
@@ -867,7 +878,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>7</v>
       </c>
@@ -890,12 +901,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1031,15 +1039,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7922E39A-5A77-4677-856B-601261C54849}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5736C62-A1D3-4E11-AF4C-44983D0C7969}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e30117fe-b212-407e-b72d-4d9fc1022dfa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1063,17 +1082,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5736C62-A1D3-4E11-AF4C-44983D0C7969}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7922E39A-5A77-4677-856B-601261C54849}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="e30117fe-b212-407e-b72d-4d9fc1022dfa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ajout des icones et fin du programme Sigfox
</commit_message>
<xml_diff>
--- a/001 - Embarquement/Identifiants.xlsx
+++ b/001 - Embarquement/Identifiants.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lacroixgroup.sharepoint.com/sites/AtelierArduinoLPWAN/Documents partages/General/LACROIX-Lab-Atelier-Arduino/001 - Embarquement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reynh\LACROIX GROUP\LACROIX GROUP\Atelier Arduino LPWAN - General\LACROIX-Lab-Atelier-Arduino\001 - Embarquement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
-  <si>
-    <t>Device EUI</t>
-  </si>
-  <si>
-    <t>a8610a30393d6d05</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Arduino</t>
   </si>
@@ -39,12 +33,6 @@
     <t>App EUI</t>
   </si>
   <si>
-    <t>50f925fb23b68de3b85a1fcf55c989de7d6a57c1</t>
-  </si>
-  <si>
-    <t>6475463840e57f1dc21360a72f14d2a1c25b2406</t>
-  </si>
-  <si>
     <t>LACROIX</t>
   </si>
   <si>
@@ -78,24 +66,6 @@
     <t>‭01100100011101010100011000111000‬</t>
   </si>
   <si>
-    <t>a8610a30393a6605</t>
-  </si>
-  <si>
-    <t>a8610a3039316905</t>
-  </si>
-  <si>
-    <t>a8610a3039246c05</t>
-  </si>
-  <si>
-    <t>a8610a30393e7205</t>
-  </si>
-  <si>
-    <t>a8610a30393f7705</t>
-  </si>
-  <si>
-    <t>a8610a30392f7805</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -148,6 +118,15 @@
   </si>
   <si>
     <t>33360EDC1EEF6D4D</t>
+  </si>
+  <si>
+    <t>50F925FB23B68DE3</t>
+  </si>
+  <si>
+    <t>Device EUI 16byte</t>
+  </si>
+  <si>
+    <t>6475463840E57F1DC21360A72F14D2A1</t>
   </si>
 </sst>
 </file>
@@ -230,14 +209,14 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,7 +257,7 @@
   <autoFilter ref="A12:B19"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Arduino"/>
-    <tableColumn id="2" name="Device EUI"/>
+    <tableColumn id="2" name="Device EUI 16byte"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -594,168 +573,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E19"/>
+  <dimension ref="A2:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.86328125" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="33.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>UPPER("50f925fb23b68de3b85a1fcf55c989de7d6a57c1")</f>
+        <v>50F925FB23B68DE3B85A1FCF55C989DE7D6A57C1</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B4" t="str">
+        <f>UPPER("6475463840e57f1dc21360a72f14d2a1c25b2406")</f>
+        <v>6475463840E57F1DC21360A72F14D2A1C25B2406</v>
+      </c>
+      <c r="C4" s="5">
+        <v>64754638</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="C10" s="7">
         <v>64754638</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="9">
-        <v>64754638</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B13" t="str">
+        <f>UPPER("a8610a30393d6d05")</f>
+        <v>A8610A30393D6D05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B14" t="str">
+        <f>UPPER("a8610a30393a6605")</f>
+        <v>A8610A30393A6605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B15" t="str">
+        <f>UPPER("a8610a3039316905")</f>
+        <v>A8610A3039316905</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B16" t="str">
+        <f>UPPER("a8610a3039246c05")</f>
+        <v>A8610A3039246C05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B17" t="str">
+        <f>UPPER("a8610a30393e7205")</f>
+        <v>A8610A30393E7205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B18" t="str">
+        <f>UPPER("a8610a30393f7705")</f>
+        <v>A8610A30393F7705</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
-      <c r="B19" t="s">
-        <v>22</v>
+      <c r="B19" t="str">
+        <f>UPPER("a8610a30392f7805")</f>
+        <v>A8610A30392F7805</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -775,121 +787,121 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -901,9 +913,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1039,26 +1054,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5736C62-A1D3-4E11-AF4C-44983D0C7969}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7922E39A-5A77-4677-856B-601261C54849}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="e30117fe-b212-407e-b72d-4d9fc1022dfa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1082,9 +1086,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7922E39A-5A77-4677-856B-601261C54849}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5736C62-A1D3-4E11-AF4C-44983D0C7969}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e30117fe-b212-407e-b72d-4d9fc1022dfa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>